<commit_message>
cleaned up the datasheet for manuscript
</commit_message>
<xml_diff>
--- a/predicted results.xlsx
+++ b/predicted results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xf290\Desktop\2019MachineLearning\Sample-Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F24523B-9C1A-421F-8039-6A25A34DD879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA05CDF-A19F-41E8-81A5-A87A1E24B60B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ea results" sheetId="1" r:id="rId1"/>
@@ -17353,7 +17353,7 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -18780,9 +18780,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EE7C5A-0766-4E5D-BFC5-E2F9D75B3141}">
   <dimension ref="A1:R111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z36" sqref="Z36"/>
+    <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21519,8 +21519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC96EC93-7E09-4340-AA85-D693148F1D24}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21677,8 +21677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDEC282-5E2C-4924-AFB6-BD1A1806D6F1}">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q53" sqref="Q53"/>
+    <sheetView zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>